<commit_message>
MA0804: Escaleta y manuscrito
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/Escaleta_MA_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/Escaleta_MA_08_04_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -1190,6 +1190,30 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1245,30 +1269,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D10" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="I1" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1608,94 +1608,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="80" t="s">
+      <c r="J1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="78" t="s">
+      <c r="K1" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="76" t="s">
+      <c r="L1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="82" t="s">
+      <c r="M1" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="82"/>
-      <c r="O1" s="70" t="s">
+      <c r="N1" s="90"/>
+      <c r="O1" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="87" t="s">
+      <c r="P1" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="89" t="s">
+      <c r="Q1" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="93" t="s">
+      <c r="R1" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="89" t="s">
+      <c r="S1" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="91" t="s">
+      <c r="T1" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="89" t="s">
+      <c r="U1" s="70" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="77"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="85"/>
       <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="71"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="94"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="90"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="71"/>
     </row>
     <row r="3" spans="1:22" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -4599,12 +4599,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4619,6 +4613,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">

</xml_diff>